<commit_message>
Se agregan diagramas de secuencia y actividades 2 SPRINT
</commit_message>
<xml_diff>
--- a/SPRINT 2/1-Planificacion/Pila del Sprint/Pila General del Sprint 2.xlsx
+++ b/SPRINT 2/1-Planificacion/Pila del Sprint/Pila General del Sprint 2.xlsx
@@ -632,18 +632,30 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -656,23 +668,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -956,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD31"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1012,58 +1012,58 @@
     </row>
     <row r="4" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="21" t="s">
+      <c r="F5" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="H5" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="24" t="s">
+      <c r="I5" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="27" t="s">
+      <c r="J5" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="28" t="s">
+      <c r="K5" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="30" t="s">
+      <c r="L5" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="20" t="s">
+      <c r="M5" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="22"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="27"/>
     </row>
     <row r="6" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="33"/>
+      <c r="B6" s="21"/>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
-      <c r="F6" s="29"/>
+      <c r="F6" s="25"/>
       <c r="G6" s="23"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="31"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="33"/>
       <c r="M6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1108,9 +1108,11 @@
       </c>
       <c r="L7" s="9">
         <f>K7-(SUM(M7:P7))</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="10">
         <v>2</v>
       </c>
-      <c r="M7" s="10"/>
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
       <c r="P7" s="11"/>
@@ -1146,9 +1148,11 @@
       </c>
       <c r="L8" s="9">
         <f t="shared" ref="L8:L31" si="0">K8-(SUM(M8:P8))</f>
+        <v>0</v>
+      </c>
+      <c r="M8" s="10">
         <v>2</v>
       </c>
-      <c r="M8" s="10"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
       <c r="P8" s="11"/>
@@ -1184,10 +1188,14 @@
       </c>
       <c r="L9" s="9">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="M9" s="10"/>
-      <c r="N9" s="6"/>
+        <v>4</v>
+      </c>
+      <c r="M9" s="10">
+        <v>2</v>
+      </c>
+      <c r="N9" s="6">
+        <v>2</v>
+      </c>
       <c r="O9" s="6"/>
       <c r="P9" s="11"/>
     </row>
@@ -1222,10 +1230,14 @@
       </c>
       <c r="L10" s="9">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="M10" s="10"/>
-      <c r="N10" s="6"/>
+        <v>4</v>
+      </c>
+      <c r="M10" s="10">
+        <v>2</v>
+      </c>
+      <c r="N10" s="6">
+        <v>2</v>
+      </c>
       <c r="O10" s="6"/>
       <c r="P10" s="11"/>
     </row>
@@ -1260,10 +1272,14 @@
       </c>
       <c r="L11" s="9">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="M11" s="10"/>
-      <c r="N11" s="6"/>
+        <v>4</v>
+      </c>
+      <c r="M11" s="10">
+        <v>2</v>
+      </c>
+      <c r="N11" s="6">
+        <v>2</v>
+      </c>
       <c r="O11" s="6"/>
       <c r="P11" s="11"/>
     </row>
@@ -1298,9 +1314,11 @@
       </c>
       <c r="L12" s="9">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="10">
         <v>10</v>
       </c>
-      <c r="M12" s="10"/>
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
       <c r="P12" s="11"/>
@@ -1336,9 +1354,11 @@
       </c>
       <c r="L13" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="M13" s="14"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="14">
+        <v>4</v>
+      </c>
       <c r="N13" s="12"/>
       <c r="O13" s="12"/>
       <c r="P13" s="15"/>
@@ -1374,10 +1394,12 @@
       </c>
       <c r="L14" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M14" s="14"/>
-      <c r="N14" s="12"/>
+      <c r="N14" s="12">
+        <v>4</v>
+      </c>
       <c r="O14" s="12"/>
       <c r="P14" s="15"/>
     </row>
@@ -1442,10 +1464,12 @@
       </c>
       <c r="L16" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M16" s="14"/>
-      <c r="N16" s="12"/>
+      <c r="N16" s="12">
+        <v>4</v>
+      </c>
       <c r="O16" s="12"/>
       <c r="P16" s="15"/>
     </row>
@@ -2037,11 +2061,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
     <mergeCell ref="M5:P5"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="H5:H6"/>
@@ -2049,6 +2068,11 @@
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="L5:L6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Se configura el 3er sprint
</commit_message>
<xml_diff>
--- a/SPRINT 2/1-Planificacion/Pila del Sprint/Pila General del Sprint 2.xlsx
+++ b/SPRINT 2/1-Planificacion/Pila del Sprint/Pila General del Sprint 2.xlsx
@@ -632,47 +632,47 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -956,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N35" sqref="N35"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1012,58 +1012,58 @@
     </row>
     <row r="4" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="22" t="s">
+      <c r="B5" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="22" t="s">
+      <c r="D5" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="28" t="s">
+      <c r="I5" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="31" t="s">
+      <c r="J5" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="24" t="s">
+      <c r="K5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="32" t="s">
+      <c r="L5" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="26" t="s">
+      <c r="M5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="N5" s="22"/>
-      <c r="O5" s="22"/>
-      <c r="P5" s="27"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="22"/>
     </row>
     <row r="6" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="21"/>
+      <c r="B6" s="33"/>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
-      <c r="F6" s="25"/>
+      <c r="F6" s="29"/>
       <c r="G6" s="23"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="33"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="31"/>
       <c r="M6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1188,7 +1188,7 @@
       </c>
       <c r="L9" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M9" s="10">
         <v>2</v>
@@ -1196,8 +1196,12 @@
       <c r="N9" s="6">
         <v>2</v>
       </c>
-      <c r="O9" s="6"/>
-      <c r="P9" s="11"/>
+      <c r="O9" s="6">
+        <v>2</v>
+      </c>
+      <c r="P9" s="11">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
@@ -1230,7 +1234,7 @@
       </c>
       <c r="L10" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M10" s="10">
         <v>2</v>
@@ -1238,8 +1242,12 @@
       <c r="N10" s="6">
         <v>2</v>
       </c>
-      <c r="O10" s="6"/>
-      <c r="P10" s="11"/>
+      <c r="O10" s="6">
+        <v>2</v>
+      </c>
+      <c r="P10" s="11">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
@@ -1272,7 +1280,7 @@
       </c>
       <c r="L11" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M11" s="10">
         <v>2</v>
@@ -1280,8 +1288,12 @@
       <c r="N11" s="6">
         <v>2</v>
       </c>
-      <c r="O11" s="6"/>
-      <c r="P11" s="11"/>
+      <c r="O11" s="6">
+        <v>2</v>
+      </c>
+      <c r="P11" s="11">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
@@ -1434,12 +1446,14 @@
       </c>
       <c r="L15" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M15" s="14"/>
       <c r="N15" s="12"/>
       <c r="O15" s="12"/>
-      <c r="P15" s="15"/>
+      <c r="P15" s="15">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
@@ -1504,12 +1518,16 @@
       </c>
       <c r="L17" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M17" s="14"/>
       <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="15"/>
+      <c r="O17" s="12">
+        <v>2</v>
+      </c>
+      <c r="P17" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="5"/>
@@ -1536,11 +1554,15 @@
       </c>
       <c r="L18" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M18" s="14"/>
-      <c r="N18" s="12"/>
-      <c r="O18" s="12"/>
+      <c r="N18" s="12">
+        <v>2</v>
+      </c>
+      <c r="O18" s="12">
+        <v>2</v>
+      </c>
       <c r="P18" s="15"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
@@ -1570,11 +1592,15 @@
       </c>
       <c r="L19" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M19" s="14"/>
-      <c r="N19" s="12"/>
-      <c r="O19" s="12"/>
+      <c r="N19" s="12">
+        <v>2</v>
+      </c>
+      <c r="O19" s="12">
+        <v>2</v>
+      </c>
       <c r="P19" s="15"/>
     </row>
     <row r="20" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
@@ -1607,11 +1633,18 @@
         <v>6</v>
       </c>
       <c r="L20" s="9">
-        <v>6</v>
-      </c>
-      <c r="M20" s="14"/>
-      <c r="N20" s="12"/>
-      <c r="O20" s="12"/>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M20" s="14">
+        <v>2</v>
+      </c>
+      <c r="N20" s="12">
+        <v>2</v>
+      </c>
+      <c r="O20" s="12">
+        <v>2</v>
+      </c>
       <c r="P20" s="15"/>
     </row>
     <row r="21" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
@@ -1645,12 +1678,14 @@
       </c>
       <c r="L21" s="9">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="M21" s="14"/>
       <c r="N21" s="12"/>
       <c r="O21" s="12"/>
-      <c r="P21" s="15"/>
+      <c r="P21" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="22" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
@@ -1683,9 +1718,11 @@
       </c>
       <c r="L22" s="9">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M22" s="14">
         <v>16</v>
       </c>
-      <c r="M22" s="14"/>
       <c r="N22" s="12"/>
       <c r="O22" s="12"/>
       <c r="P22" s="15"/>
@@ -1721,10 +1758,14 @@
       </c>
       <c r="L23" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="M23" s="14"/>
-      <c r="N23" s="12"/>
+        <v>0</v>
+      </c>
+      <c r="M23" s="14">
+        <v>2</v>
+      </c>
+      <c r="N23" s="12">
+        <v>2</v>
+      </c>
       <c r="O23" s="12"/>
       <c r="P23" s="15"/>
     </row>
@@ -1759,11 +1800,15 @@
       </c>
       <c r="L24" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M24" s="14"/>
-      <c r="N24" s="12"/>
-      <c r="O24" s="12"/>
+      <c r="N24" s="12">
+        <v>2</v>
+      </c>
+      <c r="O24" s="12">
+        <v>2</v>
+      </c>
       <c r="P24" s="15"/>
     </row>
     <row r="25" spans="2:16" ht="76.5" x14ac:dyDescent="0.25">
@@ -1797,12 +1842,16 @@
       </c>
       <c r="L25" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M25" s="14"/>
       <c r="N25" s="12"/>
-      <c r="O25" s="12"/>
-      <c r="P25" s="15"/>
+      <c r="O25" s="12">
+        <v>2</v>
+      </c>
+      <c r="P25" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="26" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
@@ -1835,12 +1884,14 @@
       </c>
       <c r="L26" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M26" s="14"/>
       <c r="N26" s="12"/>
       <c r="O26" s="12"/>
-      <c r="P26" s="15"/>
+      <c r="P26" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="27" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
@@ -1873,12 +1924,14 @@
       </c>
       <c r="L27" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M27" s="14"/>
       <c r="N27" s="12"/>
       <c r="O27" s="12"/>
-      <c r="P27" s="15"/>
+      <c r="P27" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="28" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
@@ -1911,12 +1964,14 @@
       </c>
       <c r="L28" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M28" s="14"/>
       <c r="N28" s="12"/>
       <c r="O28" s="12"/>
-      <c r="P28" s="15"/>
+      <c r="P28" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="29" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
@@ -1949,12 +2004,16 @@
       </c>
       <c r="L29" s="9">
         <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="M29" s="14"/>
+        <v>4</v>
+      </c>
+      <c r="M29" s="14">
+        <v>8</v>
+      </c>
       <c r="N29" s="12"/>
       <c r="O29" s="12"/>
-      <c r="P29" s="15"/>
+      <c r="P29" s="15">
+        <v>4</v>
+      </c>
     </row>
     <row r="30" spans="2:16" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
@@ -1987,12 +2046,14 @@
       </c>
       <c r="L30" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M30" s="14"/>
       <c r="N30" s="12"/>
       <c r="O30" s="12"/>
-      <c r="P30" s="15"/>
+      <c r="P30" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="31" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
@@ -2025,12 +2086,14 @@
       </c>
       <c r="L31" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M31" s="14"/>
       <c r="N31" s="12"/>
       <c r="O31" s="12"/>
-      <c r="P31" s="15"/>
+      <c r="P31" s="15">
+        <v>4</v>
+      </c>
     </row>
     <row r="34" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C34" s="17"/>
@@ -2061,6 +2124,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
     <mergeCell ref="M5:P5"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="H5:H6"/>
@@ -2068,11 +2136,6 @@
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="L5:L6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>